<commit_message>
Falta ver vista previa encuestas
</commit_message>
<xml_diff>
--- a/src/java/com/docenciaservicio/files/modelo docencia servicio.xlsx
+++ b/src/java/com/docenciaservicio/files/modelo docencia servicio.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oscar\Documents\NetBeansProjects\docenciaservicio\src\java\com\docenciaservicio\files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Factores" sheetId="1" r:id="rId1"/>
@@ -12,7 +17,7 @@
     <sheet name="Criterios" sheetId="3" r:id="rId3"/>
     <sheet name="Preguntas" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -467,12 +472,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -487,8 +498,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,6 +516,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -546,7 +567,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -581,7 +602,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -858,8 +879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" activeCellId="4" sqref="A10 A11 A12 A14 A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,451 +1024,664 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B54"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="145" customWidth="1"/>
+    <col min="2" max="2" width="40" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="str">
+        <f>LEFT(A2,3)</f>
+        <v>1.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C54" si="0">LEFT(A3,3)</f>
+        <v>1.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>1.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>1.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>1.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>1.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>32</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>44</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>45</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>48</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>49</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>50</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>2.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>56</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>2.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>57</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>2.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>58</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>2.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>59</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>2.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>60</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>2.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>63</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>2.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>68</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>76</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>77</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>78</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>79</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>80</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>81</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>82</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>86</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>87</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>88</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>99</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>4.1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>104</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="2" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v>4.1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>105</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v>4.1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>106</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v>4.1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>107</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>111</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="2" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39" t="str">
+        <f t="shared" si="0"/>
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>112</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40" t="str">
+        <f t="shared" si="0"/>
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>113</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41" t="str">
+        <f t="shared" si="0"/>
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>118</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="2" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42" t="str">
+        <f t="shared" si="0"/>
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>119</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43" t="str">
+        <f t="shared" si="0"/>
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>120</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="2" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44" t="str">
+        <f t="shared" si="0"/>
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>121</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="2" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45" t="str">
+        <f t="shared" si="0"/>
+        <v>4.4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>124</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="2" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46" t="str">
+        <f t="shared" si="0"/>
+        <v>4.4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>125</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="2" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47" t="str">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>130</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="2" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48" t="str">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>131</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="2" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49" t="str">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>132</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="2" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C50" t="str">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>137</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="2" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C51" t="str">
+        <f t="shared" si="0"/>
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>140</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="2" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C52" t="str">
+        <f t="shared" si="0"/>
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>141</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="2" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C53" t="str">
+        <f t="shared" si="0"/>
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>144</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="2" t="s">
         <v>143</v>
+      </c>
+      <c r="C54" t="str">
+        <f t="shared" si="0"/>
+        <v>5.2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>